<commit_message>
Dtos added + gmae functionality upgrades
</commit_message>
<xml_diff>
--- a/Tools/TestDataGeneration.xlsx
+++ b/Tools/TestDataGeneration.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Szakdolgozat\Szakdolgozat\QuizProgram_LauncherConcept\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDA149-B8E9-4B38-A5BA-BB697654BFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A2808B-E985-4241-BCF7-EADED16329C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
+    <sheet name="Topic" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="144">
   <si>
     <t>Gareth Hendricks</t>
   </si>
@@ -367,9 +368,6 @@
     <t>TeamId</t>
   </si>
   <si>
-    <t>USE [AllOrNothingDb] GO INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('</t>
-  </si>
-  <si>
     <t>Budapesti Gimi</t>
   </si>
   <si>
@@ -445,6 +443,9 @@
     <t>xd</t>
   </si>
   <si>
+    <t xml:space="preserve">) </t>
+  </si>
+  <si>
     <t>) GO</t>
   </si>
   <si>
@@ -455,6 +456,18 @@
   </si>
   <si>
     <t>Aayan Moore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USE [AllOrNothingDb] GO </t>
+  </si>
+  <si>
+    <t>INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('</t>
+  </si>
+  <si>
+    <t>USE [AllOrNothingDb] GO</t>
+  </si>
+  <si>
+    <t>INSERT INTO [dbo].[Topic] ([Name], [Description], [AuthorId] [QuestionSerieId]) VALUES('</t>
   </si>
 </sst>
 </file>
@@ -496,11 +509,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -783,27 +797,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M25" sqref="M1:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="1" max="1" width="123.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
     <col min="4" max="4" width="27.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="8.88671875" style="2"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="9" width="8.88671875" style="2"/>
-    <col min="10" max="10" width="8.88671875" style="1"/>
-    <col min="11" max="12" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="67.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="8.88671875" style="2"/>
+    <col min="11" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.88671875" style="2"/>
+    <col min="13" max="13" width="67.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>105</v>
       </c>
@@ -816,13 +834,19 @@
       <c r="H1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>109</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>99</v>
@@ -845,20 +869,23 @@
       <c r="H2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M2" s="2" t="str">
-        <f>CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2)</f>
-        <v>USE [AllOrNothingDb] GO INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Péter Árpád','Debreceni Kiss Lajos Gimnázium','Árpi',nullnull) GO</v>
+      <c r="I2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="4" t="str">
+        <f>CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2)</f>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Péter Árpád','Debreceni Kiss Lajos Gimnázium','Árpi',null,null) </v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -867,13 +894,13 @@
         <v>137</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>138</v>
@@ -881,20 +908,23 @@
       <c r="H3" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M3" s="2" t="str">
-        <f t="shared" ref="M3:M26" si="0">CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3)</f>
-        <v>USE [AllOrNothingDb] GO INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Gareth Hendricks','Budapesti Gimi','Alma',nullnull) GO</v>
+      <c r="I3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M3" s="4" t="str">
+        <f t="shared" ref="M3:M55" si="0">CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3)</f>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Gareth Hendricks','Budapesti Gimi','Alma',null,null) </v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -903,13 +933,13 @@
         <v>137</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>138</v>
@@ -917,20 +947,23 @@
       <c r="H4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>USE [AllOrNothingDb] GO INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Jamie-Leigh Banks','Atos hungray','Körte',nullnull) GO</v>
+      <c r="I4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Jamie-Leigh Banks','Atos hungray','Körte',null,null) </v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>139</v>
@@ -939,13 +972,13 @@
         <v>137</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>138</v>
@@ -953,20 +986,23 @@
       <c r="H5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>USE [AllOrNothingDb] GO INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Aayan Moore','Bosch Gmbh','Banán',nullnull) GO</v>
+      <c r="I5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Aayan Moore','Bosch Gmbh','Banán',null,null) </v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -975,13 +1011,13 @@
         <v>137</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>138</v>
@@ -989,20 +1025,23 @@
       <c r="H6" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>USE [AllOrNothingDb] GO INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Kajol Peralta','Apple','Eper',nullnull) GO</v>
+      <c r="I6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Kajol Peralta','Apple','Eper',null,null) </v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -1011,13 +1050,13 @@
         <v>137</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>138</v>
@@ -1025,18 +1064,24 @@
       <c r="H7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>USE [AllOrNothingDb] GO INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Baran Neale','Google','Dinnye',nullnull) GO</v>
+      <c r="I7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Baran Neale','Google','Dinnye',null,null) </v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1044,13 +1089,13 @@
         <v>137</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>138</v>
@@ -1058,18 +1103,24 @@
       <c r="H8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gavin Clemons','Microsoft','Kiwi',nullnull) GO</v>
+      <c r="I8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Gavin Clemons','Microsoft','Kiwi',null,null) </v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1077,13 +1128,13 @@
         <v>137</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>138</v>
@@ -1091,18 +1142,24 @@
       <c r="H9" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Dustin Clifford','RiotGames','Szőlő',nullnull) GO</v>
+      <c r="I9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Dustin Clifford','RiotGames','Szőlő',null,null) </v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1110,13 +1167,13 @@
         <v>137</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>138</v>
@@ -1124,18 +1181,24 @@
       <c r="H10" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Reeva Broughton','PSEG','Mandarin',nullnull) GO</v>
+      <c r="I10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Reeva Broughton','PSEG','Mandarin',null,null) </v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1143,13 +1206,13 @@
         <v>137</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>138</v>
@@ -1157,18 +1220,24 @@
       <c r="H11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Kaitlyn Sims','Hidasi Általános Iskola','Narancs',nullnull) GO</v>
+      <c r="I11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Kaitlyn Sims','Hidasi Általános Iskola','Narancs',null,null) </v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1176,13 +1245,13 @@
         <v>137</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>138</v>
@@ -1190,18 +1259,24 @@
       <c r="H12" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Matthias Bolton','Elte','Mazsola',nullnull) GO</v>
+      <c r="I12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Matthias Bolton','Elte','Mazsola',null,null) </v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1209,13 +1284,13 @@
         <v>137</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>138</v>
@@ -1223,18 +1298,24 @@
       <c r="H13" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Indiana Mendez','ELTE IK','Maracuja',nullnull) GO</v>
+      <c r="I13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Indiana Mendez','ELTE IK','Maracuja',null,null) </v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1242,13 +1323,13 @@
         <v>137</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>138</v>
@@ -1256,18 +1337,24 @@
       <c r="H14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Imaad Dodson','ELTE BGGYK','Montenegró',nullnull) GO</v>
+      <c r="I14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Imaad Dodson','ELTE BGGYK','Montenegró',null,null) </v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1278,7 +1365,7 @@
         <v>137</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>138</v>
@@ -1286,18 +1373,24 @@
       <c r="H15" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Eugene Medrano','','xd',nullnull) GO</v>
+      <c r="I15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Eugene Medrano','','xd',null,null) </v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1313,18 +1406,24 @@
       <c r="H16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Nial Stubbs','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Nial Stubbs','','',null,null) </v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1340,18 +1439,24 @@
       <c r="H17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Huzaifa Brett','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Huzaifa Brett','','',null,null) </v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1367,18 +1472,24 @@
       <c r="H18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Aurora Fisher','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Aurora Fisher','','',null,null) </v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1394,18 +1505,24 @@
       <c r="H19" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Karishma Johnston','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Karishma Johnston','','',null,null) </v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1421,18 +1538,24 @@
       <c r="H20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Aarav Kelly','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Aarav Kelly','','',null,null) </v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
@@ -1448,18 +1571,24 @@
       <c r="H21" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Shani Southern','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Shani Southern','','',null,null) </v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
@@ -1475,18 +1604,24 @@
       <c r="H22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Rhiannan Vincent','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Rhiannan Vincent','','',null,null) </v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
@@ -1502,18 +1637,24 @@
       <c r="H23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Kyran Glover','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Kyran Glover','','',null,null) </v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1529,18 +1670,24 @@
       <c r="H24" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Christie Nelson','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Christie Nelson','','',null,null) </v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
@@ -1556,18 +1703,24 @@
       <c r="H25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Margie Hubbard','','',nullnull) GO</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M25" s="4" t="str">
+        <f>CONCATENATE(A25,B25,C25,D25,E25,F25,G25,H25,I25,J25,K25)</f>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Margie Hubbard','','',null,null) </v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
@@ -1580,15 +1733,21 @@
       <c r="G26" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Mylah Ratcliffe','','',) GO</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Mylah Ratcliffe','','',,) </v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
@@ -1601,11 +1760,21 @@
       <c r="G27" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Alana Bennett,'','',,) </v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
@@ -1618,11 +1787,21 @@
       <c r="G28" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Jennie Wilson,'','',,) </v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
@@ -1635,11 +1814,21 @@
       <c r="G29" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Meghan Jensen,','',,) </v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
@@ -1652,11 +1841,21 @@
       <c r="G30" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Miah Mason,','',,) </v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
@@ -1669,11 +1868,21 @@
       <c r="G31" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Fathima Wagstaff,','',,) </v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
@@ -1686,11 +1895,21 @@
       <c r="G32" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Alishba Garner,','',,) </v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>29</v>
       </c>
@@ -1703,11 +1922,21 @@
       <c r="G33" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Emily Corrigan,','',,) </v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B34" s="2" t="s">
         <v>30</v>
       </c>
@@ -1720,11 +1949,18 @@
       <c r="G34" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">INSERT INTO [dbo].[Players] ([Name] ,[Institue] ,[NickName] ,[QuestionSerieId] ,[TeamId]) VALUES ('Nichola Meza,','',,) </v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>31</v>
       </c>
@@ -1737,11 +1973,18 @@
       <c r="G35" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Emily-Jane Mcfarland,','',,) </v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>32</v>
       </c>
@@ -1754,11 +1997,18 @@
       <c r="G36" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Alasdair Beck,','',,) </v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
@@ -1771,11 +2021,18 @@
       <c r="G37" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Beyonce Griffith,','',,) </v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>34</v>
       </c>
@@ -1788,11 +2045,18 @@
       <c r="G38" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Connie Walker,','',,) </v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
@@ -1805,11 +2069,18 @@
       <c r="G39" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Zakir Anthony,','',,) </v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
@@ -1822,11 +2093,18 @@
       <c r="G40" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Hallam Mcdougall,','',,) </v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>37</v>
       </c>
@@ -1839,11 +2117,18 @@
       <c r="G41" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Harper Bate,','',,) </v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>38</v>
       </c>
@@ -1856,11 +2141,18 @@
       <c r="G42" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Emerson Galindo,','',,) </v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>39</v>
       </c>
@@ -1873,11 +2165,18 @@
       <c r="G43" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Tanya Gutierrez,','',,) </v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
@@ -1890,11 +2189,18 @@
       <c r="G44" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Dante Broadhurst,','',,) </v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
@@ -1907,11 +2213,18 @@
       <c r="G45" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Mohammad Whiteley,','',,) </v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
@@ -1924,11 +2237,18 @@
       <c r="G46" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Juan Watkins,','',,) </v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>43</v>
       </c>
@@ -1941,11 +2261,18 @@
       <c r="G47" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Zakariya Gale,','',,) </v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>44</v>
       </c>
@@ -1958,11 +2285,18 @@
       <c r="G48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Sebastian Childs,',',,) </v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
         <v>45</v>
       </c>
@@ -1975,11 +2309,18 @@
       <c r="G49" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Tasmin Thompson,',',,) </v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>46</v>
       </c>
@@ -1992,11 +2333,18 @@
       <c r="G50" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M50" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Collette Whyte,',',,) </v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
         <v>47</v>
       </c>
@@ -2009,11 +2357,18 @@
       <c r="G51" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I51" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M51" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Dawud Mclellan,',',,) </v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>48</v>
       </c>
@@ -2026,11 +2381,18 @@
       <c r="G52" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M52" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Abdurahman Tait,',',,) </v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
         <v>49</v>
       </c>
@@ -2043,11 +2405,18 @@
       <c r="G53" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M53" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Sacha Redman,',',,) </v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
         <v>50</v>
       </c>
@@ -2060,11 +2429,18 @@
       <c r="G54" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I54" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M54" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Stephanie Wilkerson,',',,) </v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
         <v>51</v>
       </c>
@@ -2077,11 +2453,18 @@
       <c r="G55" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M55" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Elinor Mendoza,',',,) </v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
         <v>52</v>
       </c>
@@ -2094,11 +2477,14 @@
       <c r="G56" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I56" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>53</v>
       </c>
@@ -2111,11 +2497,14 @@
       <c r="G57" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
         <v>54</v>
       </c>
@@ -2128,11 +2517,14 @@
       <c r="G58" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I58" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
         <v>55</v>
       </c>
@@ -2145,11 +2537,14 @@
       <c r="G59" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J59" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I59" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
         <v>56</v>
       </c>
@@ -2162,11 +2557,14 @@
       <c r="G60" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I60" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
         <v>57</v>
       </c>
@@ -2179,11 +2577,14 @@
       <c r="G61" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J61" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I61" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
         <v>58</v>
       </c>
@@ -2196,11 +2597,14 @@
       <c r="G62" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I62" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
         <v>59</v>
       </c>
@@ -2213,11 +2617,14 @@
       <c r="G63" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I63" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>60</v>
       </c>
@@ -2230,11 +2637,14 @@
       <c r="G64" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I64" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>61</v>
       </c>
@@ -2247,11 +2657,14 @@
       <c r="G65" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J65" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I65" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>62</v>
       </c>
@@ -2264,11 +2677,14 @@
       <c r="G66" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J66" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I66" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>63</v>
       </c>
@@ -2281,11 +2697,14 @@
       <c r="G67" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J67" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I67" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
         <v>64</v>
       </c>
@@ -2298,11 +2717,14 @@
       <c r="G68" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I68" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>65</v>
       </c>
@@ -2315,11 +2737,14 @@
       <c r="G69" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I69" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>66</v>
       </c>
@@ -2332,11 +2757,14 @@
       <c r="G70" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J70" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I70" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
         <v>67</v>
       </c>
@@ -2349,11 +2777,14 @@
       <c r="G71" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J71" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I71" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
         <v>68</v>
       </c>
@@ -2366,11 +2797,14 @@
       <c r="G72" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J72" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
         <v>69</v>
       </c>
@@ -2383,11 +2817,14 @@
       <c r="G73" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J73" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
         <v>70</v>
       </c>
@@ -2400,11 +2837,14 @@
       <c r="G74" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I74" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
         <v>71</v>
       </c>
@@ -2417,11 +2857,14 @@
       <c r="G75" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J75" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I75" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
         <v>72</v>
       </c>
@@ -2434,11 +2877,14 @@
       <c r="G76" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J76" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I76" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>73</v>
       </c>
@@ -2451,11 +2897,14 @@
       <c r="G77" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J77" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I77" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>74</v>
       </c>
@@ -2468,11 +2917,14 @@
       <c r="G78" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J78" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I78" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>75</v>
       </c>
@@ -2485,11 +2937,14 @@
       <c r="G79" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J79" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I79" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>76</v>
       </c>
@@ -2502,11 +2957,14 @@
       <c r="G80" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J80" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I80" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
         <v>77</v>
       </c>
@@ -2519,11 +2977,14 @@
       <c r="G81" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J81" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I81" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
         <v>78</v>
       </c>
@@ -2536,11 +2997,14 @@
       <c r="G82" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J82" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I82" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
         <v>79</v>
       </c>
@@ -2553,11 +3017,14 @@
       <c r="G83" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J83" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I83" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>80</v>
       </c>
@@ -2570,11 +3037,14 @@
       <c r="G84" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J84" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I84" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>81</v>
       </c>
@@ -2587,11 +3057,14 @@
       <c r="G85" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J85" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I85" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B86" s="2" t="s">
         <v>82</v>
       </c>
@@ -2604,11 +3077,14 @@
       <c r="G86" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J86" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I86" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
         <v>83</v>
       </c>
@@ -2621,11 +3097,14 @@
       <c r="G87" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J87" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I87" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
         <v>84</v>
       </c>
@@ -2638,11 +3117,14 @@
       <c r="G88" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J88" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I88" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
         <v>85</v>
       </c>
@@ -2655,11 +3137,14 @@
       <c r="G89" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J89" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I89" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>86</v>
       </c>
@@ -2672,11 +3157,14 @@
       <c r="G90" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J90" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>87</v>
       </c>
@@ -2689,11 +3177,14 @@
       <c r="G91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J91" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I91" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>88</v>
       </c>
@@ -2706,11 +3197,14 @@
       <c r="G92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J92" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I92" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B93" s="2" t="s">
         <v>89</v>
       </c>
@@ -2723,11 +3217,14 @@
       <c r="G93" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J93" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I93" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
         <v>90</v>
       </c>
@@ -2740,11 +3237,14 @@
       <c r="G94" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J94" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I94" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B95" s="2" t="s">
         <v>91</v>
       </c>
@@ -2757,11 +3257,14 @@
       <c r="G95" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J95" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I95" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B96" s="2" t="s">
         <v>92</v>
       </c>
@@ -2774,11 +3277,14 @@
       <c r="G96" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J96" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I96" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B97" s="2" t="s">
         <v>93</v>
       </c>
@@ -2791,11 +3297,14 @@
       <c r="G97" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J97" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I97" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B98" s="2" t="s">
         <v>94</v>
       </c>
@@ -2808,11 +3317,14 @@
       <c r="G98" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J98" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I98" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B99" s="2" t="s">
         <v>95</v>
       </c>
@@ -2825,11 +3337,14 @@
       <c r="G99" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J99" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I99" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B100" s="2" t="s">
         <v>96</v>
       </c>
@@ -2842,11 +3357,14 @@
       <c r="G100" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J100" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I100" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B101" s="2" t="s">
         <v>97</v>
       </c>
@@ -2859,11 +3377,14 @@
       <c r="G101" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J101" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I101" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B102" s="2" t="s">
         <v>98</v>
       </c>
@@ -2872,10 +3393,44 @@
       </c>
       <c r="G102" s="3" t="s">
         <v>103</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4688C37-9D4F-4642-814C-F0D4E74EE2D4}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>